<commit_message>
svg scale sample viewbox
</commit_message>
<xml_diff>
--- a/src/App_DevResources/Device-resolutions.xlsx
+++ b/src/App_DevResources/Device-resolutions.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Documents\_Data\GitHub\azure-samples\blazor-samples\src\App_DevResources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF10FA1-89D7-4252-B454-20020E60BDF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="14370" windowHeight="12045" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample-Resolutions" sheetId="1" r:id="rId1"/>
@@ -13,7 +19,7 @@
     <sheet name="Words" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -792,7 +798,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1183,18 +1189,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C19" sqref="C19:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1733,11 +1739,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,11 +1819,11 @@
         <v>3088</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D16" si="0">B2/C2</f>
+        <f t="shared" ref="D2:D18" si="0">B2/C2</f>
         <v>0.46632124352331605</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E16" si="1">MIN(C2, B2)</f>
+        <f t="shared" ref="E2:E18" si="1">MIN(C2, B2)</f>
         <v>1440</v>
       </c>
       <c r="F2">
@@ -1845,11 +1851,11 @@
         <v>0.1</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M16" si="2">B2*L2</f>
+        <f t="shared" ref="M2:M18" si="2">B2*L2</f>
         <v>144</v>
       </c>
       <c r="N2">
-        <f t="shared" ref="N2:N16" si="3">C2*L2</f>
+        <f t="shared" ref="N2:N18" si="3">C2*L2</f>
         <v>308.8</v>
       </c>
     </row>
@@ -2076,7 +2082,7 @@
         <v>100</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G16" si="7">D7*F7</f>
+        <f t="shared" ref="G7:G18" si="7">D7*F7</f>
         <v>160</v>
       </c>
       <c r="H7">
@@ -2440,14 +2446,14 @@
         <v>0.1</v>
       </c>
       <c r="I14">
-        <f t="shared" ref="I14:I16" si="8">(E14*H14) / 100</f>
+        <f t="shared" ref="I14:I18" si="8">(E14*H14) / 100</f>
         <v>0.36</v>
       </c>
       <c r="J14">
         <v>1</v>
       </c>
       <c r="K14">
-        <f t="shared" ref="K14:K16" si="9">F14*I14*J14</f>
+        <f t="shared" ref="K14:K18" si="9">F14*I14*J14</f>
         <v>36</v>
       </c>
       <c r="L14">
@@ -2558,7 +2564,103 @@
         <v>184.8</v>
       </c>
     </row>
-    <row r="31" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1170</v>
+      </c>
+      <c r="C17">
+        <v>2532</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.46208530805687204</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>1170</v>
+      </c>
+      <c r="F17">
+        <v>100</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="7"/>
+        <v>46.208530805687204</v>
+      </c>
+      <c r="H17">
+        <v>0.1</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="8"/>
+        <v>1.17</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="9"/>
+        <v>117</v>
+      </c>
+      <c r="L17">
+        <v>0.1</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="3"/>
+        <v>253.20000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1848</v>
+      </c>
+      <c r="C18">
+        <v>2960</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0.62432432432432428</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>1848</v>
+      </c>
+      <c r="F18">
+        <v>100</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="7"/>
+        <v>62.432432432432428</v>
+      </c>
+      <c r="H18">
+        <v>0.1</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="8"/>
+        <v>1.8480000000000001</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="9"/>
+        <v>184.8</v>
+      </c>
+      <c r="L18">
+        <v>0.1</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="2"/>
+        <v>184.8</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="3"/>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J31" t="s">
         <v>217</v>
       </c>
@@ -2569,7 +2671,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -3484,7 +3586,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D60">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D60">
     <sortCondition descending="1" ref="D1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3492,7 +3594,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3555,7 +3657,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>